<commit_message>
SDK_The Vision & The TimeLine SDK_SysCtrl.0x01
</commit_message>
<xml_diff>
--- a/the SDK Vision.xlsx
+++ b/the SDK Vision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>APP_LAYER</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>sticks</t>
+  </si>
+  <si>
+    <t>BY:</t>
+  </si>
+  <si>
+    <t>Game Console</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -496,26 +502,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -540,31 +553,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,38 +881,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="33">
+      <c r="E1" s="18"/>
+      <c r="F1" s="14">
         <v>43474</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="14"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="11"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
@@ -940,8 +940,10 @@
       <c r="K2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="L2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="16"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -953,9 +955,9 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="8"/>
@@ -977,33 +979,33 @@
       <c r="T3" s="3"/>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="32"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="13"/>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="29"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1023,9 +1025,9 @@
       <c r="T5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="30"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1045,9 +1047,9 @@
       <c r="T6" s="7"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="29" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="31" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="4"/>
@@ -1069,9 +1071,9 @@
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="29"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1091,9 +1093,9 @@
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="30"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1113,10 +1115,10 @@
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1155,9 +1157,9 @@
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="8"/>
@@ -1181,35 +1183,35 @@
       <c r="T11" s="3"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="32"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="13"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="29"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="4" t="s">
         <v>43</v>
       </c>
@@ -1231,9 +1233,9 @@
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="30"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1253,8 +1255,8 @@
       <c r="T14" s="7"/>
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="28" t="s">
         <v>32</v>
       </c>
@@ -1277,9 +1279,9 @@
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1299,9 +1301,9 @@
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="30"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1321,10 +1323,10 @@
       <c r="T17" s="5"/>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="18"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
         <v>20</v>
       </c>
@@ -1369,9 +1371,9 @@
       <c r="T18" s="3"/>
     </row>
     <row r="19" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="10" t="s">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="8"/>
@@ -1393,33 +1395,33 @@
       <c r="T19" s="3"/>
     </row>
     <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="32"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1439,9 +1441,9 @@
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1461,8 +1463,8 @@
       <c r="T22" s="7"/>
     </row>
     <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="28" t="s">
         <v>32</v>
       </c>
@@ -1485,9 +1487,9 @@
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="29"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="31"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1507,9 +1509,9 @@
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="29"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="31"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1529,9 +1531,9 @@
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="30"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1551,10 +1553,10 @@
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
         <v>20</v>
       </c>
@@ -1609,9 +1611,9 @@
       <c r="T27" s="3"/>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="10" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="8"/>
@@ -1633,8 +1635,8 @@
       <c r="T28" s="3"/>
     </row>
     <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="28" t="s">
         <v>32</v>
       </c>
@@ -1657,9 +1659,9 @@
       <c r="T29" s="5"/>
     </row>
     <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="29"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1679,9 +1681,9 @@
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="29"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1701,9 +1703,9 @@
       <c r="T31" s="5"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="30"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1723,11 +1725,13 @@
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="11"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1747,9 +1751,11 @@
       <c r="T33" s="3"/>
     </row>
     <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="11"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1769,9 +1775,9 @@
       <c r="T34" s="5"/>
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="12"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -1791,7 +1797,17 @@
       <c r="T35" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="A27:B32"/>
+    <mergeCell ref="A33:B35"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A18:B26"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -1800,17 +1816,9 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A2:B9"/>
     <mergeCell ref="A10:B17"/>
-    <mergeCell ref="A18:B26"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="L10:M10"/>
-    <mergeCell ref="A27:B32"/>
-    <mergeCell ref="A33:B35"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>